<commit_message>
Added periods to exclude from GAGE
</commit_message>
<xml_diff>
--- a/data/data_selection/data_combination.xlsx
+++ b/data/data_selection/data_combination.xlsx
@@ -8,12 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chxmr/code/agage-archive/data/data_selection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7564175-ECE2-3446-AB2E-CD06F3645D43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4159C10B-4BF5-A141-8C38-30C72F362178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2880" yWindow="2560" windowWidth="27240" windowHeight="16440" xr2:uid="{9985A75E-EB26-5749-BA8E-B1A91FE63120}"/>
   </bookViews>
   <sheets>
     <sheet name="CGO" sheetId="1" r:id="rId1"/>
+    <sheet name="MHD" sheetId="2" r:id="rId2"/>
+    <sheet name="THD" sheetId="3" r:id="rId3"/>
+    <sheet name="RPB" sheetId="4" r:id="rId4"/>
+    <sheet name="SMO" sheetId="5" r:id="rId5"/>
+    <sheet name="ZEP" sheetId="6" r:id="rId6"/>
+    <sheet name="CMN" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -63,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="29">
   <si>
     <t># File specifying when to use the various ALE/GAGE/AGAGE instruments</t>
   </si>
@@ -156,7 +162,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -171,12 +177,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -738,4 +738,616 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC29711F-13B8-9140-B473-D8767E35D5EB}">
+  <dimension ref="A1:Q8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="10.83203125" style="1"/>
+    <col min="3" max="3" width="15.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="15.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5" style="1" customWidth="1"/>
+    <col min="10" max="10" width="17.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="17" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{160591D1-02F5-5E4D-B7FE-18CBFE4B0D82}">
+  <dimension ref="A1:Q8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="10.83203125" style="1"/>
+    <col min="3" max="3" width="15.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="15.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5" style="1" customWidth="1"/>
+    <col min="10" max="10" width="17.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="17" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95CA49D9-7FA7-1249-B393-DC69D0A3EC82}">
+  <dimension ref="A1:Q8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="10.83203125" style="1"/>
+    <col min="3" max="3" width="15.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="15.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5" style="1" customWidth="1"/>
+    <col min="10" max="10" width="17.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="17" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C45BA512-5AE4-3C4F-BEFD-5BBCD1F01554}">
+  <dimension ref="A1:Q8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="10.83203125" style="1"/>
+    <col min="3" max="3" width="15.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="15.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5" style="1" customWidth="1"/>
+    <col min="10" max="10" width="17.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="17" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C42BA6F3-6164-0740-9787-95981F3E2AF1}">
+  <dimension ref="A1:Q8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="10.83203125" style="1"/>
+    <col min="3" max="3" width="15.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="15.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5" style="1" customWidth="1"/>
+    <col min="10" max="10" width="17.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="17" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{282330B1-5456-C947-8C60-CDB83BC163C1}">
+  <dimension ref="A1:Q8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="10.83203125" style="1"/>
+    <col min="3" max="3" width="15.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="15.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5" style="1" customWidth="1"/>
+    <col min="10" max="10" width="17.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="17" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>